<commit_message>
add the model for approve leave link.
</commit_message>
<xml_diff>
--- a/Learnings/Learnings.xlsx
+++ b/Learnings/Learnings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Technology</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Devise tutorials (Devise is a gem)</t>
+  </si>
+  <si>
+    <t>http://twitter.github.com/bootstrap/javascript.html#tabs</t>
+  </si>
+  <si>
+    <t>active menu</t>
   </si>
 </sst>
 </file>
@@ -426,6 +432,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="15" spans="1:4">
       <c r="C15" s="1"/>
     </row>

</xml_diff>

<commit_message>
implement the pagination for user index page and leave index page.
</commit_message>
<xml_diff>
--- a/Learnings/Learnings.xlsx
+++ b/Learnings/Learnings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Technology</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>active menu</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/13222406/undefined-method-current-page-for-array0x007fd5ef6dd158-kaminari</t>
+  </si>
+  <si>
+    <t>undifind method 'current_page' for array kaminari gem.</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,6 +444,17 @@
       </c>
       <c r="C4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>